<commit_message>
changed adapter PCB to cheaper made with partial through hole design
</commit_message>
<xml_diff>
--- a/pcb/BOM_BlueSmart_vedirect_PCB_BlueSmart_vedirect.xlsx
+++ b/pcb/BOM_BlueSmart_vedirect_PCB_BlueSmart_vedirect.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="BOM_BlueSmart_vedirect_PCB_Blue" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="BOM_Board1_PCB1_2023-09-22" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -109,19 +109,19 @@
     <t>4</t>
   </si>
   <si>
-    <t>VE.direct</t>
-  </si>
-  <si>
-    <t>VE.D1</t>
-  </si>
-  <si>
-    <t>CONN-SMD_PH2.0-4PWB</t>
-  </si>
-  <si>
-    <t>BOOMELE(博穆精密)</t>
-  </si>
-  <si>
-    <t>C50137</t>
+    <t>HDGC2001WR-4P</t>
+  </si>
+  <si>
+    <t>VE.DIRECT1</t>
+  </si>
+  <si>
+    <t>CONN-TH_4P-P2.00_HDGC_HDGC2001WR-4P</t>
+  </si>
+  <si>
+    <t>HDGC(华德共创)</t>
+  </si>
+  <si>
+    <t>C5175241</t>
   </si>
 </sst>
 </file>

</xml_diff>